<commit_message>
adding next papers to read
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezy/Desktop/Spring 2025/Computer-Vision-Papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4D98F2-1105-174C-978E-065F84617D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344321B8-59C8-1E47-BC85-C1D0D92C58E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" activeTab="1" xr2:uid="{DFDC9FC7-5844-914B-A846-75D92E17BE5E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{DFDC9FC7-5844-914B-A846-75D92E17BE5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Medical" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="272">
   <si>
     <t>AUTHOR</t>
   </si>
@@ -1061,6 +1061,143 @@
   </si>
   <si>
     <t>https://arxiv.org/abs/2403.13523</t>
+  </si>
+  <si>
+    <t>Emegining Properties in Self-Supervised vision Transformers (DINO Paper)</t>
+  </si>
+  <si>
+    <t>Mathilde Caron et al.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2104.14294</t>
+  </si>
+  <si>
+    <t>MIMIC-CXR, a de-identified publicly available database of chest radiographs with free-text reports (MIMIC_CXR Dataset)</t>
+  </si>
+  <si>
+    <t>Algorithmic Fairness in Lesion Classification by Mitigating Class Imbalance and Skin Tone Bias</t>
+  </si>
+  <si>
+    <t>Faizanuddin Ansari et al.</t>
+  </si>
+  <si>
+    <t>https://papers.miccai.org/miccai-2024/059-Paper2178.html</t>
+  </si>
+  <si>
+    <t>CheXplaining in Style: Counterfactual Explanations for Chest X-rays using StyleGAN</t>
+  </si>
+  <si>
+    <t>Matan Atad.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2207.07553</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This paper introduces a fully convolutional masked autoencoder framework and a new Global Response Normalization (GRN) layer that can be added to the ConvNeXt architecture to enhance inter-channel feature competition. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ConvNeXt are considered modern ConvNet architectures (modern CNNs).  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Their model scored 76.7% top-1 accuracy on ImageNet, to a 650M Huge model that achieves a state-of-theart 88.9% accuracy using only public training data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This paper tackles several issues. (1) Leverage MAE architectures for downstream tasks is not trivial.  MAE has a specific encode-decoder design that is optimized for the sequence processing capabilities of transformers, which allows the compute-heavy encoder to focus on visible patches and thus reduce the pre-training cost. (2) A potential issue of feature collapse at the MLP layer when training ConvNeXt directly on masked input. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>In response they added a  Global Response Normalization layer to enhance inter-channel feature competition.</t>
+    </r>
+  </si>
+  <si>
+    <t>ConvNeXt V2: Co-designing and Scaling ConvNets with Masked Autoencoders</t>
+  </si>
+  <si>
+    <t>Sanghyun Woo et al.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2301.00808</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TURBOFUZZLLM:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Turbocharging Mutation-based Fuzzing for Effectively Jailbreaking Large Language Models in Practice</t>
+    </r>
+  </si>
+  <si>
+    <t>Aman Goel et al.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2502.18504</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FuzzLLM: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Novel and Universal Fuzzing Framework for Proactively Discovering Jailbreak Vulnerabilities in Large Language Models</t>
+    </r>
+  </si>
+  <si>
+    <t>Dongyu Yao et al.</t>
+  </si>
+  <si>
+    <t>ICASSP</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10448041?denied=</t>
   </si>
 </sst>
 </file>
@@ -1488,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0739E5-9D2D-3840-A96D-0B4389A2B83F}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A8" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1794,6 +1931,23 @@
         <v>130</v>
       </c>
     </row>
+    <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2022</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
     <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>86</v>
@@ -1907,6 +2061,7 @@
     <hyperlink ref="E3" r:id="rId13" xr:uid="{6EBBF2C7-9C86-534F-A9CC-1461A7688687}"/>
     <hyperlink ref="E2" r:id="rId14" xr:uid="{30C26C86-7E56-4943-8A7D-3BB89D4D2DDD}"/>
     <hyperlink ref="E11" r:id="rId15" xr:uid="{F9D99B05-6B59-F34A-8603-32274C3F4A2D}"/>
+    <hyperlink ref="E12" r:id="rId16" xr:uid="{C5E8F719-4D2D-A749-8B85-EC2EC6FABE86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1916,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A226E7A5-1AE7-2D4A-8771-BC3D7E1CAFD3}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2560,38 +2715,134 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="221" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2025</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2024</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C31" s="3">
         <v>2024</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="32" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C32" s="3">
         <v>2024</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2024</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2680,8 +2931,13 @@
     <hyperlink ref="E22" r:id="rId24" xr:uid="{CB424513-FC41-424D-AAA2-E3209FB3A6C8}"/>
     <hyperlink ref="E23" r:id="rId25" xr:uid="{5833EA3A-86DB-E746-9088-625E6CD42AF1}"/>
     <hyperlink ref="E24" r:id="rId26" xr:uid="{3AFFB290-C1F7-5F4E-B244-8B33EDC805E9}"/>
-    <hyperlink ref="E25" r:id="rId27" xr:uid="{F4B3227E-C0BB-F041-8E3D-AF69D4257333}"/>
-    <hyperlink ref="E26" r:id="rId28" xr:uid="{3FFD2720-E2F3-D44F-B20D-66DCE42054B3}"/>
+    <hyperlink ref="E31" r:id="rId27" xr:uid="{F4B3227E-C0BB-F041-8E3D-AF69D4257333}"/>
+    <hyperlink ref="E32" r:id="rId28" xr:uid="{3FFD2720-E2F3-D44F-B20D-66DCE42054B3}"/>
+    <hyperlink ref="E33" r:id="rId29" xr:uid="{4A48CE80-D16F-2A4A-8153-CEF41EBF4F81}"/>
+    <hyperlink ref="E35" r:id="rId30" xr:uid="{0DBD99FC-278A-504D-920E-9D94804FCA0F}"/>
+    <hyperlink ref="E25" r:id="rId31" xr:uid="{73C97F82-9250-3645-8804-75424EABAF3D}"/>
+    <hyperlink ref="E26" r:id="rId32" xr:uid="{1FF8CA26-E284-5241-9062-F9C797A71FA2}"/>
+    <hyperlink ref="E27" r:id="rId33" xr:uid="{0AB4E0C4-E072-0A4F-ADFD-8C9ED96C56C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding more papers to csv
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezy/Desktop/Spring 2025/Computer-Vision-Papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344321B8-59C8-1E47-BC85-C1D0D92C58E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B46F6-326A-3549-992B-F3A0CAB22D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{DFDC9FC7-5844-914B-A846-75D92E17BE5E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17080" windowHeight="20400" activeTab="1" xr2:uid="{DFDC9FC7-5844-914B-A846-75D92E17BE5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Medical" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="275">
   <si>
     <t>AUTHOR</t>
   </si>
@@ -1198,6 +1198,15 @@
   </si>
   <si>
     <t>https://ieeexplore.ieee.org/document/10448041?denied=</t>
+  </si>
+  <si>
+    <t>Focused on jailbreak vulnerabilities in LLMs, this paper creates a framework called FuzzLLM to proactively test and discover jailbreak vulnerabilities in LLMs.  They introduce templates (which capture structural integrity) and contraints (key features of the jailbreak) to enable efficient testing with reduced manual efforts.</t>
+  </si>
+  <si>
+    <t>(1) FuzzLLM Framework (2) adoption of fuzzing whic employ black-box fuzzing for insightful asssessments without accessing the mode's intricate details (3) Prompt generation strategy and (4) comprehensive evaluation eight distinct LLMs</t>
+  </si>
+  <si>
+    <t>Jailbreaking/ Security</t>
   </si>
 </sst>
 </file>
@@ -2071,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A226E7A5-1AE7-2D4A-8771-BC3D7E1CAFD3}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="75" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2754,8 +2763,11 @@
       <c r="E26" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="H26" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>268</v>
       </c>
@@ -2771,6 +2783,16 @@
       <c r="E27" s="4" t="s">
         <v>271</v>
       </c>
+      <c r="F27" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="I27" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">

</xml_diff>

<commit_message>
adding transformers without normalization
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezy/Desktop/Spring 2025/Computer-Vision-Papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC596C03-7529-214A-B2A0-DF8943C4C1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8366E1D8-6E2E-B542-BB6C-1F6642CA187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28560" windowHeight="20380" activeTab="1" xr2:uid="{DFDC9FC7-5844-914B-A846-75D92E17BE5E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{DFDC9FC7-5844-914B-A846-75D92E17BE5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Medical" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="289">
   <si>
     <t>AUTHOR</t>
   </si>
@@ -1225,6 +1225,30 @@
   </si>
   <si>
     <t>https://arxiv.org/abs/1805.07932</t>
+  </si>
+  <si>
+    <t>Transformers without Normalization</t>
+  </si>
+  <si>
+    <t>Jiachen Zhu et al.</t>
+  </si>
+  <si>
+    <t>https://jiachenzhu.github.io/DyT/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In attempts to introduce a more efficient attention mechanism, this paper proposes bilinear attention networks which are features </t>
+  </si>
+  <si>
+    <t>(1) low-rank bilinear pooling for combining questions vector and multi-channel input image. (2) Bilinear attention network which improves upon previously used bilinear models.</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Jiachen Zhu et al., challenges pre-existing normalization methods employed in state-of-the art attention-based deep learning models. Specifically, they demonstrate how layer normalization layers exhibit similar behaviors as tanh functions. This papers proves this theory and demonstrates that we can achieve similar performance  accross numerous deep learning models (e.g. DiT, ViT, and ConvNeXt) by replacing  LN layers with proposed Dynamic tanh (DyT)layers. They also showcase that DyT decreases LLaMA 7B inference (7.8%) and training (8.2%) times.</t>
+  </si>
+  <si>
+    <t>(1) Discussed the purpose of layer normalization and their visual Tanh-like behavior. (2) provided pseudocode implementations for DyT. (3)Evaluated the efficiency of DyT in comparison to root mean square normalization layers. (4) Provided a series of ablation studies (i.e. replacing tanh with hard tanh and sigmoid)</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0739E5-9D2D-3840-A96D-0B4389A2B83F}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="171" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2109,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A226E7A5-1AE7-2D4A-8771-BC3D7E1CAFD3}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="75" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2823,7 +2847,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>278</v>
       </c>
@@ -2838,6 +2862,41 @@
       </c>
       <c r="E28" s="3" t="s">
         <v>280</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="221" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -3007,6 +3066,7 @@
     <hyperlink ref="E26" r:id="rId32" xr:uid="{1FF8CA26-E284-5241-9062-F9C797A71FA2}"/>
     <hyperlink ref="E27" r:id="rId33" xr:uid="{0AB4E0C4-E072-0A4F-ADFD-8C9ED96C56C4}"/>
     <hyperlink ref="E28" r:id="rId34" xr:uid="{CC66DD93-4F16-A346-9639-CB723A4F5EAB}"/>
+    <hyperlink ref="E29" r:id="rId35" xr:uid="{DE665102-F824-CE4C-A630-C4C4D7034EDB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
read byte latent transformer paper
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezy/Desktop/Spring 2025/Computer-Vision-Papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8366E1D8-6E2E-B542-BB6C-1F6642CA187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27072395-56EE-B647-A294-9FDC24125B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{DFDC9FC7-5844-914B-A846-75D92E17BE5E}"/>
+    <workbookView xWindow="35260" yWindow="1780" windowWidth="20580" windowHeight="25520" activeTab="1" xr2:uid="{DFDC9FC7-5844-914B-A846-75D92E17BE5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Medical" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="295">
   <si>
     <t>AUTHOR</t>
   </si>
@@ -1249,13 +1249,50 @@
   </si>
   <si>
     <t>(1) Discussed the purpose of layer normalization and their visual Tanh-like behavior. (2) provided pseudocode implementations for DyT. (3)Evaluated the efficiency of DyT in comparison to root mean square normalization layers. (4) Provided a series of ablation studies (i.e. replacing tanh with hard tanh and sigmoid)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ByteLatentTransformer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: PatchesScaleBetter ThanTokens</t>
+    </r>
+  </si>
+  <si>
+    <t>Artidoro Pagnoni et al.</t>
+  </si>
+  <si>
+    <t>https://ai.meta.com/research/publications/byte-latent-transformer-patches-scale-better-than-tokens/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This paper introduces byte latent transformer (BLT) that improves the scaling trends of LLMs. Operating in the byte space is costly due to long sequence lengths. Previous methods have explored more efficient attention mechanisms and remove attention all together. BLT is dynamic and learnable method for grouping bytes  into patchs (a patch-based approach). One unique difference between this method and other patch methods is that BLT has no fixed size or vocabulary for patches. </t>
+  </si>
+  <si>
+    <t>(1) BLT, byte latent LLM architecture that dynamically allocates compute to improve FLOP (floating point operations per seconds) (2) Unlocking a new dimension of scaling LLMs . (3) Authors demonstrate imporved robustness of BLT models to input noise and awareness of sub-word aspects</t>
+  </si>
+  <si>
+    <t>LLMs/ Architecture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1674,7 +1711,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="26" style="2" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" style="2" customWidth="1"/>
@@ -1688,7 +1725,7 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1714,7 +1751,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="129" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="129" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>118</v>
       </c>
@@ -1740,7 +1777,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="182" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="182" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>111</v>
       </c>
@@ -1766,7 +1803,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="187">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1795,7 +1832,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="204">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1821,7 +1858,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="187">
       <c r="A6" s="2" t="s">
         <v>82</v>
       </c>
@@ -1847,7 +1884,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="187">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -1873,7 +1910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="136">
       <c r="A8" s="2" t="s">
         <v>70</v>
       </c>
@@ -1899,7 +1936,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="204">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -1925,7 +1962,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="221" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="221">
       <c r="A10" s="2" t="s">
         <v>98</v>
       </c>
@@ -1954,7 +1991,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="136">
       <c r="A11" s="2" t="s">
         <v>125</v>
       </c>
@@ -1977,7 +2014,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="68">
       <c r="A12" s="2" t="s">
         <v>256</v>
       </c>
@@ -1994,7 +2031,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="51">
       <c r="A13" s="2" t="s">
         <v>273</v>
       </c>
@@ -2011,7 +2048,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="51">
       <c r="A30" s="2" t="s">
         <v>86</v>
       </c>
@@ -2028,7 +2065,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="68">
       <c r="A31" s="2" t="s">
         <v>90</v>
       </c>
@@ -2045,7 +2082,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="68">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -2065,7 +2102,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="102">
       <c r="A33" s="2" t="s">
         <v>13</v>
       </c>
@@ -2085,7 +2122,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="102">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -2133,11 +2170,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A226E7A5-1AE7-2D4A-8771-BC3D7E1CAFD3}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="38" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="32" style="2" customWidth="1"/>
@@ -2150,7 +2187,7 @@
     <col min="9" max="9" width="43.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="28">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2176,7 +2213,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="102">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2202,7 +2239,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="102">
       <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
@@ -2228,7 +2265,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="119">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
@@ -2254,7 +2291,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="102">
       <c r="A5" s="2" t="s">
         <v>93</v>
       </c>
@@ -2280,7 +2317,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="119">
       <c r="A6" s="4" t="s">
         <v>218</v>
       </c>
@@ -2306,7 +2343,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="136">
       <c r="A7" s="4" t="s">
         <v>219</v>
       </c>
@@ -2332,7 +2369,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="119">
       <c r="A8" s="4" t="s">
         <v>217</v>
       </c>
@@ -2358,7 +2395,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="136">
       <c r="A9" s="2" t="s">
         <v>135</v>
       </c>
@@ -2384,7 +2421,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="136">
       <c r="A10" s="4" t="s">
         <v>220</v>
       </c>
@@ -2410,7 +2447,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="187" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="187">
       <c r="A11" s="2" t="s">
         <v>145</v>
       </c>
@@ -2436,7 +2473,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="102">
       <c r="A12" s="2" t="s">
         <v>150</v>
       </c>
@@ -2462,7 +2499,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="136">
       <c r="A13" s="2" t="s">
         <v>156</v>
       </c>
@@ -2488,7 +2525,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="170">
       <c r="A14" s="2" t="s">
         <v>180</v>
       </c>
@@ -2514,7 +2551,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="170">
       <c r="A15" s="2" t="s">
         <v>157</v>
       </c>
@@ -2540,7 +2577,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="153">
       <c r="A16" s="2" t="s">
         <v>179</v>
       </c>
@@ -2566,7 +2603,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="204">
       <c r="A17" s="2" t="s">
         <v>181</v>
       </c>
@@ -2592,7 +2629,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="340" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="340">
       <c r="A18" s="2" t="s">
         <v>187</v>
       </c>
@@ -2618,7 +2655,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="289" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="289">
       <c r="A19" s="4" t="s">
         <v>221</v>
       </c>
@@ -2647,7 +2684,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="255" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="255">
       <c r="A20" s="4" t="s">
         <v>222</v>
       </c>
@@ -2673,7 +2710,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="136">
       <c r="A21" s="4" t="s">
         <v>223</v>
       </c>
@@ -2699,7 +2736,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="136">
       <c r="A22" s="2" t="s">
         <v>224</v>
       </c>
@@ -2725,7 +2762,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="255" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="255">
       <c r="A23" s="2" t="s">
         <v>231</v>
       </c>
@@ -2751,7 +2788,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="306" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="306">
       <c r="A24" s="2" t="s">
         <v>236</v>
       </c>
@@ -2777,7 +2814,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="221" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="221">
       <c r="A25" s="2" t="s">
         <v>260</v>
       </c>
@@ -2800,7 +2837,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="85">
       <c r="A26" s="4" t="s">
         <v>263</v>
       </c>
@@ -2820,7 +2857,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="136">
       <c r="A27" s="4" t="s">
         <v>266</v>
       </c>
@@ -2847,7 +2884,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="75" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>278</v>
       </c>
@@ -2873,7 +2910,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="221" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="221">
       <c r="A29" s="2" t="s">
         <v>281</v>
       </c>
@@ -2899,7 +2936,33 @@
         <v>286</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="187">
+      <c r="A30" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="85">
       <c r="A31" s="2" t="s">
         <v>242</v>
       </c>
@@ -2916,7 +2979,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="51">
       <c r="A32" s="2" t="s">
         <v>245</v>
       </c>
@@ -2933,7 +2996,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="51">
       <c r="A33" s="2" t="s">
         <v>249</v>
       </c>
@@ -2950,12 +3013,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="85">
       <c r="A34" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="68">
       <c r="A35" s="2" t="s">
         <v>253</v>
       </c>
@@ -2972,7 +3035,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="34">
       <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
@@ -2989,7 +3052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="34">
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
@@ -3003,7 +3066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="102">
       <c r="A40" s="4" t="s">
         <v>12</v>
       </c>
@@ -3017,12 +3080,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="17">
       <c r="A41" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="51">
       <c r="A42" s="2" t="s">
         <v>106</v>
       </c>
@@ -3067,6 +3130,7 @@
     <hyperlink ref="E27" r:id="rId33" xr:uid="{0AB4E0C4-E072-0A4F-ADFD-8C9ED96C56C4}"/>
     <hyperlink ref="E28" r:id="rId34" xr:uid="{CC66DD93-4F16-A346-9639-CB723A4F5EAB}"/>
     <hyperlink ref="E29" r:id="rId35" xr:uid="{DE665102-F824-CE4C-A630-C4C4D7034EDB}"/>
+    <hyperlink ref="E30" r:id="rId36" xr:uid="{634A3153-FC32-224E-B177-95F5D0763A41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>